<commit_message>
tamamlandi - ama read timeout problemini coz
</commit_message>
<xml_diff>
--- a/csbBirimFiyat/1.xlsx
+++ b/csbBirimFiyat/1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>701-101</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>MONTAJ</t>
+  </si>
+  <si>
+    <t>708-100</t>
+  </si>
+  <si>
+    <t>SAÇ, DOLAP TİPİ ANA TABLOLAR (TS EN 61439-1/2 )</t>
+  </si>
+  <si>
+    <t>708-101</t>
+  </si>
+  <si>
+    <t>SAC DOLAP TiPi ANA TAB.30x30x40 cm.GÖZ (TS EN 61439-1/2 )</t>
   </si>
 </sst>
 </file>
@@ -69,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,12 +89,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,6 +471,32 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>